<commit_message>
Se mejora la visualización de resultados
</commit_message>
<xml_diff>
--- a/code/resultados.xlsx
+++ b/code/resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,18 +456,18 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[PDF][PDF] Mapa de la vulnerabilidad socioeconómica en la ciudad de Luján (Buenos Aires, Argentina) a partir de la metodología del Valor de Índice Medio</t>
+          <t>[PDF][PDF] Medio ambiente</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.researchgate.net/profile/Noelia-Principi/publication/341610976_Mapa_de_la_vulnerabilidad_socioeconomica_en_la_ciudad_de_Lujan_Buenos_Aires_Argentina_a_partir_de_la_metodologia_del_Valor_de_Indice_Medio/links/5ecac92b299bf1c09adcd419/Mapa-de-la-vulnerabilidad-socioeconomica-en-la-ciudad-de-Lujan-Buenos-Aires-Argentina-a-partir-de-la-metodologia-del-Valor-de-Indice-Medio.pdf</t>
+          <t>http://revista.humanidades.unam.mx/revista_32/revista_32_tema06.pdf</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>… of socioeconomic vulnerability conditions in the city of Luján (Buenos Aires, Argentina). The 
-… distribution of the socioeconomic vulnerability in the city of Luján. As a line of advance, a …</t>
+          <t>… ambiental.“En dicha cumbre se acordaron medidas para la protección del medio ambiente. 
+… , en el cual se demanda la integración del medio ambiente y el desarrollo económico”. Este …</t>
         </is>
       </c>
     </row>
@@ -477,18 +477,18 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[PDF][PDF] Distribución y segregación espacial de los extranjeros en la Ciudad de Luján. Un Análisis según la Geografía Cuantitativa.</t>
+          <t>[PDF][PDF] Medio ambiente</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://p3.usal.edu.ar/index.php/signos/article/download/2229/2777</t>
+          <t>https://we.riseup.net/assets/279881/Problemas+ambientales.pdf</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>… Está formado por los 43 radios censales urbanos en que se divide la ciudad de Luján (Figura 
-1) y por los mapas temáticos surgidos de la totalidad de variables (Figuras 2 a 8), …</t>
+          <t>Medio ambiente … 4 Medio ambiente/José Luis Lezama y Boris Graizbord, coordinadores-1a. 
+ed.--México, DF: El Colegio de México, 2010 429 p.; 22 cm.--… Los temas que se abordan …</t>
         </is>
       </c>
     </row>
@@ -498,18 +498,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[PDF][PDF] Centro histórico de la ciudad de Luján, provincia de Buenos Aires</t>
+          <t>[PDF][PDF] Medio ambiente y desarrollo</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>http://mail.eure.cl/index.php/eure/article/view/1131/233</t>
+          <t>https://repositorio.cepal.org/server/api/core/bitstreams/a799dbd6-22cd-4351-9a8f-83a4270da732/content</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>… de Luján, coordinado por Margarita Gutman, Jorge Enrique Hardoy y Giorgio Piccinato, 
-que se encuentra preparado para su publicación por la Universidad Nacional de Luján. La …</t>
+          <t>Este documento fue preparado por Ricardo Vicari, consultor de la Unidad de Políticas para 
+el Desarrollo Sostenible de la División de Desarrollo Sostenible y Asentamientos Humanos …</t>
         </is>
       </c>
     </row>
@@ -519,18 +519,18 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[PDF][PDF] EL MAPA SOCIAL DE LA CIUDAD DE LUJÁN EN 1991, 2001 y 2010. Un modelo espacial consolidado.</t>
+          <t>[PDF][PDF] Desarrollo y medio ambiente: una mirada a Colombia</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.researchgate.net/profile/Gustavo-Buzai/publication/296706632_El_mapa_social_de_la_ciudad_de_Lujan_en_1991_2001_y_2010_Un_modelo_espacial_consolidado/links/56d9fa5308aebe4638bb9dc3/El-mapa-social-de-la-ciudad-de-Lujan-en-1991-2001-y-2010-Un-modelo-espacial-consolidado.pdf</t>
+          <t>https://guao.org/sites/default/files/biblioteca/Desarrollo%20y%20medio%20ambiente%20una%20mirada%20a%20Colombia.pdf</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>… El presente trabajo, valiéndose de estos recursos analiza los mapas sociales de la ciudad 
-de Luján en 1991, 2001 y 2010, lo cual demuestra que el modelo espacial de la ciudad se …</t>
+          <t>… ha afectado y afecta el medio ambiente. En Colombia, como … e influye en el medio ambiente 
+y los recursos naturales. Así, … le estamos dando y daremos al medio ambiente; es nuestra …</t>
         </is>
       </c>
     </row>
@@ -540,18 +540,81 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[PDF][PDF] Mapa social y vulnerabilidad socioeconómica en la ciudad de Luján, Buenos Aires, Argentina</t>
+          <t>[PDF][PDF] Medio ambiente urbano</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.researchgate.net/profile/Jose-Aparicio-Lopez/publication/352506052_Diagnostico_socioambiental_participativo_en_una_comunidad_rural_el_caso_de_Texca_Guerrero/links/62b9e314056dae24e8e75913/Diagnostico-socioambiental-participativo-en-una-comunidad-rural-el-caso-de-Texca-Guerrero.pdf#page=18</t>
+          <t>https://www.redalyc.org/pdf/1694/169414452002.pdf</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>El capítulo presenta el análisis de las condiciones socioespaciales urbanas en la ciudad de 
-Luján, a partir de la determinación de la relación existente entre el mapa social y la …</t>
+          <t>… Medio Ambiente y Desarrollo, con el propósito de orientar la reflexión conjunta sobre la 
+situación en América Latina respecto de las relaciones entre el ambiente y … temática ambiental a …</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>[PDF][PDF] Vulnerabilidad y medio ambiente</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.buyteknet.info/fileshare/data/ana_pla_sis_amb/Vul_medio%20ambiente.pdf</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>… entre medio ambiente y sociedad el planteamiento tradicional ha sido el de evaluación 
+de impacto, es decir, se selecciona algo que puede generar cambios en el medio ambiente (…</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>[PDF][PDF] Plásticos y medio ambiente</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.academia.edu/download/59214400/REVISTA_SOBRE_PLASTICOS20190511-120589-1ic8uu6.pdf</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>… nocivos que acarrean al medio ambiente y por ende a la vida… revolución trascendente para 
+el medio ambiente, y hasta … medio ambiente”, por que aún no se les puede considerar como …</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>[PDF][PDF] Ambiente y el Desarrollo</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://archivoteologicogranadino.uloyola.es/rfs/article/download/2810/1355</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>… Los Estados deberán promulgar leyes efectivas sobre el medio ambiente. Las normas 
+ambientales y los objetivos y prioridades en materia de gestión del medio ambiente, deberían …</t>
         </is>
       </c>
     </row>

</xml_diff>